<commit_message>
Further data descriptions added and a short presentation of the different answers has been added.
</commit_message>
<xml_diff>
--- a/pigw21s.xlsx
+++ b/pigw21s.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:HC43"/>
+  <dimension ref="A1:GX43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1396,31 +1396,6 @@
           <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : Other (please specify)</t>
         </is>
       </c>
-      <c r="GY1" s="1" t="inlineStr">
-        <is>
-          <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : What is the name of your institution/organisation?</t>
-        </is>
-      </c>
-      <c r="GZ1" s="1" t="inlineStr">
-        <is>
-          <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : What is the name of your school/department?</t>
-        </is>
-      </c>
-      <c r="HA1" s="1" t="inlineStr">
-        <is>
-          <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : What is your current tenure status?</t>
-        </is>
-      </c>
-      <c r="HB1" s="1" t="inlineStr">
-        <is>
-          <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : Which country/ territory are you located in?</t>
-        </is>
-      </c>
-      <c r="HC1" s="1" t="inlineStr">
-        <is>
-          <t>In this final section we would like to understand a little about you specifically to again provide additional context to previous responses given. : Thank you very much for completing this survey. If you are willing to be contacted in case of follow up questions please put your e-mail address in the field below. All contact details will be deleted upon the completion of the project.</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1429,28 +1404,20 @@
         </is>
       </c>
       <c r="B2">
-        <v>256081511</v>
+        <v>257953342</v>
       </c>
       <c r="C2" s="2">
-        <v>44462.62475694445</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44470.31486111111</v>
+        <v>44452.40900462963</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1989</t>
-        </is>
-      </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ANR</t>
+          <t>public local government</t>
         </is>
       </c>
       <c r="L2">
@@ -1758,25 +1725,33 @@
         </is>
       </c>
       <c r="B3">
-        <v>256002708</v>
+        <v>256572231</v>
       </c>
       <c r="C3" s="2">
-        <v>44455.55599537037</v>
+        <v>44452.89104166666</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44468.41116898148</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Life sciences</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Institute</t>
+          <t>Gobernamental institution</t>
         </is>
       </c>
       <c r="J3">
@@ -2126,23 +2101,6 @@
       </c>
       <c r="GW3">
         <v>3</v>
-      </c>
-      <c r="GY3" t="inlineStr">
-        <is>
-          <t>Research Institute for Farm Animal Biology (FBN)</t>
-        </is>
-      </c>
-      <c r="GZ3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Institute of Nutritional Physiology "Oskar Kellner" _x000D_
-</t>
-        </is>
-      </c>
-      <c r="HA3">
-        <v>1</v>
-      </c>
-      <c r="HB3">
-        <v>65</v>
       </c>
     </row>
     <row r="4">
@@ -2152,28 +2110,28 @@
         </is>
       </c>
       <c r="B4">
-        <v>257622269</v>
+        <v>256002708</v>
       </c>
       <c r="C4" s="2">
-        <v>44469.90278935185</v>
+        <v>44452.50744212963</v>
       </c>
       <c r="D4" s="2">
-        <v>44455.56491898149</v>
+        <v>44454.68528935185</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
       <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Animal Sciences</t>
-        </is>
+        <v>2</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Public funder</t>
+          <t>government</t>
         </is>
       </c>
       <c r="J4">
@@ -2283,33 +2241,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>255999250</v>
+        <v>257634686</v>
       </c>
       <c r="C5" s="2">
-        <v>44452.89104166666</v>
+        <v>44467.72662037037</v>
       </c>
       <c r="D5" s="2">
-        <v>44469.91393518518</v>
+        <v>44452.63277777778</v>
       </c>
       <c r="E5">
         <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1989</t>
-        </is>
       </c>
       <c r="G5">
         <v>12</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Animal health</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>private foundations</t>
+          <t>German Research Foundation (DFG)_x000D_
+EU_x000D_
+German Federal Ministry for Research and Education (BMBF)</t>
         </is>
       </c>
       <c r="J5">
@@ -2350,28 +2300,33 @@
         </is>
       </c>
       <c r="B6">
-        <v>256108088</v>
+        <v>257626415</v>
       </c>
       <c r="C6" s="2">
-        <v>44463.86545138889</v>
+        <v>44470.30331018519</v>
       </c>
       <c r="D6" s="2">
-        <v>44455.46233796296</v>
+        <v>44483.6057175926</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Animal Science</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>private companies</t>
+          <t>Agroscope, Europe (via ITN)</t>
         </is>
       </c>
       <c r="J6">
@@ -2637,22 +2592,6 @@
       </c>
       <c r="GW6">
         <v>3</v>
-      </c>
-      <c r="GY6" t="inlineStr">
-        <is>
-          <t>Research Institute for Farm Animal Biology</t>
-        </is>
-      </c>
-      <c r="GZ6" t="inlineStr">
-        <is>
-          <t>Institute of Behavioural Physiology</t>
-        </is>
-      </c>
-      <c r="HA6">
-        <v>1</v>
-      </c>
-      <c r="HB6">
-        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -2662,28 +2601,23 @@
         </is>
       </c>
       <c r="B7">
-        <v>256278995</v>
+        <v>258024220</v>
       </c>
       <c r="C7" s="2">
         <v>44456.43879629629</v>
       </c>
       <c r="D7" s="2">
-        <v>44455.46857638888</v>
+        <v>44470.74857638888</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>12</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>European commision</t>
+          <t>Private companies</t>
         </is>
       </c>
       <c r="J7">
@@ -2970,22 +2904,6 @@
       </c>
       <c r="GW7">
         <v>3</v>
-      </c>
-      <c r="GY7" t="inlineStr">
-        <is>
-          <t>Research Institute for Farm Animal Biology</t>
-        </is>
-      </c>
-      <c r="GZ7" t="inlineStr">
-        <is>
-          <t>Institute for Behavioural Physiology</t>
-        </is>
-      </c>
-      <c r="HA7">
-        <v>2</v>
-      </c>
-      <c r="HB7">
-        <v>65</v>
       </c>
     </row>
     <row r="8">
@@ -2995,28 +2913,28 @@
         </is>
       </c>
       <c r="B8">
-        <v>257620376</v>
+        <v>255977069</v>
       </c>
       <c r="C8" s="2">
-        <v>44477.46344907407</v>
+        <v>44456.50266203703</v>
       </c>
       <c r="D8" s="2">
-        <v>44452.63277777778</v>
+        <v>44456.45372685185</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
       <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>veterinary medicine</t>
-        </is>
+        <v>12</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>DFG</t>
+          <t>I work at a publicly funded research institute, with additional funding mostly from the DFG and EU.</t>
         </is>
       </c>
       <c r="J8">
@@ -3304,22 +3222,6 @@
       </c>
       <c r="GW8">
         <v>1</v>
-      </c>
-      <c r="GY8" t="inlineStr">
-        <is>
-          <t>Wageningen University</t>
-        </is>
-      </c>
-      <c r="GZ8" t="inlineStr">
-        <is>
-          <t>Animal Sciences</t>
-        </is>
-      </c>
-      <c r="HA8">
-        <v>3</v>
-      </c>
-      <c r="HB8">
-        <v>123</v>
       </c>
     </row>
     <row r="9">
@@ -3329,28 +3231,33 @@
         </is>
       </c>
       <c r="B9">
-        <v>257131420</v>
+        <v>258842562</v>
       </c>
       <c r="C9" s="2">
-        <v>44467.67416666666</v>
+        <v>44476.61056712962</v>
       </c>
       <c r="D9" s="2">
-        <v>44452.52055555556</v>
+        <v>44454.530625</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Animal Sciences</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>The Danish Veterinary and Food Administration</t>
+          <t>My research institute</t>
         </is>
       </c>
       <c r="J9">
@@ -3613,12 +3520,6 @@
       </c>
       <c r="GW9">
         <v>3</v>
-      </c>
-      <c r="HA9">
-        <v>5</v>
-      </c>
-      <c r="HB9">
-        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -3628,23 +3529,28 @@
         </is>
       </c>
       <c r="B10">
-        <v>257936554</v>
+        <v>256361947</v>
       </c>
       <c r="C10" s="2">
-        <v>44455.36075231481</v>
+        <v>44455.4534375</v>
       </c>
       <c r="D10" s="2">
         <v>44452.67950231482</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
       </c>
       <c r="G10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>my institute and Europe programs</t>
+          <t>Europe Funds</t>
         </is>
       </c>
       <c r="J10">
@@ -3925,25 +3831,6 @@
       </c>
       <c r="GW10">
         <v>3</v>
-      </c>
-      <c r="GY10" t="inlineStr">
-        <is>
-          <t>INRAE</t>
-        </is>
-      </c>
-      <c r="GZ10" t="inlineStr">
-        <is>
-          <t>Animal Genetics</t>
-        </is>
-      </c>
-      <c r="HA10">
-        <v>1</v>
-      </c>
-      <c r="HB10">
-        <v>61</v>
-      </c>
-      <c r="HC10">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -3953,28 +3840,28 @@
         </is>
       </c>
       <c r="B11">
-        <v>258842562</v>
+        <v>256278995</v>
       </c>
       <c r="C11" s="2">
-        <v>44467.66538194445</v>
+        <v>44455.55667824074</v>
       </c>
       <c r="D11" s="2">
-        <v>44467.72538194444</v>
+        <v>44455.41337962963</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2008</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>public local government</t>
+          <t>private foundations</t>
         </is>
       </c>
       <c r="J11">
@@ -4282,25 +4169,6 @@
       </c>
       <c r="GW11">
         <v>3</v>
-      </c>
-      <c r="GY11" t="inlineStr">
-        <is>
-          <t>Agroscope</t>
-        </is>
-      </c>
-      <c r="GZ11" t="inlineStr">
-        <is>
-          <t>Animal Production Systems and Animal Health</t>
-        </is>
-      </c>
-      <c r="HA11">
-        <v>1</v>
-      </c>
-      <c r="HB11">
-        <v>170</v>
-      </c>
-      <c r="HC11">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -4310,13 +4178,13 @@
         </is>
       </c>
       <c r="B12">
-        <v>257948090</v>
+        <v>256064531</v>
       </c>
       <c r="C12" s="2">
-        <v>44468.39248842592</v>
+        <v>44467.65707175925</v>
       </c>
       <c r="D12" s="2">
-        <v>44470.74857638888</v>
+        <v>44468.38256944445</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -4329,9 +4197,14 @@
       <c r="G12">
         <v>12</v>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Veterinary Epidemiology</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>Goverment</t>
         </is>
       </c>
       <c r="J12">
@@ -4493,26 +4366,6 @@
         <v>2</v>
       </c>
       <c r="GW12">
-        <v>1</v>
-      </c>
-      <c r="GY12" t="inlineStr">
-        <is>
-          <t>Aarhus University</t>
-        </is>
-      </c>
-      <c r="GZ12" t="inlineStr">
-        <is>
-          <t>Department of Animal Science (main place of work)_x000D_
-Bioinformatics Research Centre (affiliation/secondary place of work)</t>
-        </is>
-      </c>
-      <c r="HA12">
-        <v>1</v>
-      </c>
-      <c r="HB12">
-        <v>47</v>
-      </c>
-      <c r="HC12">
         <v>1</v>
       </c>
     </row>
@@ -4523,20 +4376,17 @@
         </is>
       </c>
       <c r="B13">
-        <v>258024220</v>
+        <v>256362038</v>
       </c>
       <c r="C13" s="2">
-        <v>44455.44020833333</v>
-      </c>
-      <c r="D13" s="2">
-        <v>44456.51704861112</v>
+        <v>44452.68103009259</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="G13">
@@ -4544,7 +4394,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>National research instute for my salary and europe for my research</t>
+          <t>European commision</t>
         </is>
       </c>
       <c r="J13">
@@ -4816,22 +4666,6 @@
       </c>
       <c r="GW13">
         <v>3</v>
-      </c>
-      <c r="GY13" t="inlineStr">
-        <is>
-          <t>INRAE</t>
-        </is>
-      </c>
-      <c r="GZ13" t="inlineStr">
-        <is>
-          <t>PEGASE</t>
-        </is>
-      </c>
-      <c r="HA13">
-        <v>1</v>
-      </c>
-      <c r="HB13">
-        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -4841,24 +4675,29 @@
         </is>
       </c>
       <c r="B14">
-        <v>256542441</v>
+        <v>257622269</v>
       </c>
       <c r="C14" s="2">
-        <v>44470.73622685185</v>
+        <v>44455.36075231481</v>
       </c>
       <c r="D14" s="2">
-        <v>44467.74414351852</v>
+        <v>44453.79085648149</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Rennes Metropole and #DIGITAG</t>
+        </is>
       </c>
       <c r="J14">
         <v>1</v>
@@ -5126,25 +4965,6 @@
       </c>
       <c r="GW14">
         <v>3</v>
-      </c>
-      <c r="GY14" t="inlineStr">
-        <is>
-          <t>FBN</t>
-        </is>
-      </c>
-      <c r="GZ14" t="inlineStr">
-        <is>
-          <t>Nutritional Physiology</t>
-        </is>
-      </c>
-      <c r="HA14">
-        <v>1</v>
-      </c>
-      <c r="HB14">
-        <v>65</v>
-      </c>
-      <c r="HC14">
-        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -5154,28 +4974,30 @@
         </is>
       </c>
       <c r="B15">
-        <v>256572231</v>
+        <v>258745041</v>
       </c>
       <c r="C15" s="2">
-        <v>44467.65707175925</v>
-      </c>
-      <c r="D15" s="2">
-        <v>44455.41337962963</v>
+        <v>44453.3491550926</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
       <c r="G15">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Statistics and mathematics</t>
+          <t>Animal nutrient</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Starting grant</t>
+          <t>Gouverment and economy</t>
         </is>
       </c>
       <c r="J15">
@@ -5435,12 +5257,6 @@
       </c>
       <c r="GW15">
         <v>3</v>
-      </c>
-      <c r="HA15">
-        <v>1</v>
-      </c>
-      <c r="HB15">
-        <v>65</v>
       </c>
     </row>
     <row r="16">
@@ -5450,24 +5266,29 @@
         </is>
       </c>
       <c r="B16">
-        <v>257689731</v>
+        <v>256324567</v>
       </c>
       <c r="C16" s="2">
-        <v>44470.34854166667</v>
+        <v>44467.65208333333</v>
       </c>
       <c r="D16" s="2">
-        <v>44453.79085648149</v>
+        <v>44452.52055555556</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>1996</t>
         </is>
       </c>
       <c r="G16">
         <v>2</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>State.</t>
+        </is>
       </c>
       <c r="J16">
         <v>1</v>
@@ -5738,22 +5559,6 @@
       </c>
       <c r="GW16">
         <v>3</v>
-      </c>
-      <c r="GY16" t="inlineStr">
-        <is>
-          <t>The French National Research Institute for Agriculture, Food, and the Environment (INRAE)</t>
-        </is>
-      </c>
-      <c r="GZ16" t="inlineStr">
-        <is>
-          <t>Human Nutrition department</t>
-        </is>
-      </c>
-      <c r="HA16">
-        <v>1</v>
-      </c>
-      <c r="HB16">
-        <v>61</v>
       </c>
     </row>
     <row r="17">
@@ -5763,17 +5568,20 @@
         </is>
       </c>
       <c r="B17">
-        <v>256026620</v>
+        <v>255999250</v>
       </c>
       <c r="C17" s="2">
-        <v>44452.40900462963</v>
+        <v>44461.74114583334</v>
+      </c>
+      <c r="D17" s="2">
+        <v>44461.79481481481</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2003</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="G17">
@@ -5781,14 +5589,12 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Veterinary Epidemiology</t>
+          <t>Animal nutrition</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>German Research Foundation (DFG)_x000D_
-EU_x000D_
-German Federal Ministry for Research and Education (BMBF)</t>
+          <t>University funding</t>
         </is>
       </c>
       <c r="J17">
@@ -5971,14 +5777,6 @@
       </c>
       <c r="GW17">
         <v>3</v>
-      </c>
-      <c r="GY17" t="inlineStr">
-        <is>
-          <t>Agroscope</t>
-        </is>
-      </c>
-      <c r="HB17">
-        <v>170</v>
       </c>
     </row>
     <row r="18">
@@ -5988,17 +5786,20 @@
         </is>
       </c>
       <c r="B18">
-        <v>256171924</v>
+        <v>255998073</v>
       </c>
       <c r="C18" s="2">
-        <v>44452.52850694444</v>
+        <v>44455.55599537037</v>
+      </c>
+      <c r="D18" s="2">
+        <v>44452.68805555555</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="G18">
@@ -6006,7 +5807,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Gouverment and economy</t>
+          <t>The German Government</t>
         </is>
       </c>
       <c r="L18">
@@ -6277,22 +6078,6 @@
       </c>
       <c r="GW18">
         <v>4</v>
-      </c>
-      <c r="GY18" t="inlineStr">
-        <is>
-          <t>Agroscope</t>
-        </is>
-      </c>
-      <c r="GZ18" t="inlineStr">
-        <is>
-          <t>Swine nutrition</t>
-        </is>
-      </c>
-      <c r="HA18">
-        <v>5</v>
-      </c>
-      <c r="HB18">
-        <v>170</v>
       </c>
     </row>
     <row r="19">
@@ -6302,30 +6087,28 @@
         </is>
       </c>
       <c r="B19">
-        <v>257626517</v>
+        <v>257681865</v>
       </c>
       <c r="C19" s="2">
-        <v>44453.78319444445</v>
+        <v>44454.66171296296</v>
+      </c>
+      <c r="D19" s="2">
+        <v>44467.67511574074</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>1995</t>
         </is>
       </c>
       <c r="G19">
-        <v>12</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Agriculture</t>
-        </is>
+        <v>2</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Gobernamental institution</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J19">
@@ -6564,22 +6347,6 @@
       </c>
       <c r="GW19">
         <v>1</v>
-      </c>
-      <c r="GY19" t="inlineStr">
-        <is>
-          <t>Aarhus University</t>
-        </is>
-      </c>
-      <c r="GZ19" t="inlineStr">
-        <is>
-          <t>Animal Science</t>
-        </is>
-      </c>
-      <c r="HA19">
-        <v>3</v>
-      </c>
-      <c r="HB19">
-        <v>47</v>
       </c>
     </row>
     <row r="20">
@@ -6589,33 +6356,28 @@
         </is>
       </c>
       <c r="B20">
-        <v>257040687</v>
+        <v>256032817</v>
       </c>
       <c r="C20" s="2">
-        <v>44461.74114583334</v>
+        <v>44463.86545138889</v>
       </c>
       <c r="D20" s="2">
-        <v>44454.68528935185</v>
+        <v>44455.56491898149</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
       <c r="G20">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Animal nutrient</t>
+          <t>Agriculture</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>The Swiss government</t>
+          <t>Swedish Research Council FORMAS</t>
         </is>
       </c>
       <c r="J20">
@@ -6857,22 +6619,6 @@
       </c>
       <c r="GW20">
         <v>1</v>
-      </c>
-      <c r="GY20" t="inlineStr">
-        <is>
-          <t>Animal Science</t>
-        </is>
-      </c>
-      <c r="GZ20" t="inlineStr">
-        <is>
-          <t>Animal nutrition and physiology</t>
-        </is>
-      </c>
-      <c r="HA20">
-        <v>3</v>
-      </c>
-      <c r="HB20">
-        <v>47</v>
       </c>
     </row>
     <row r="21">
@@ -6882,33 +6628,33 @@
         </is>
       </c>
       <c r="B21">
-        <v>256337741</v>
+        <v>256108088</v>
       </c>
       <c r="C21" s="2">
-        <v>44453.3491550926</v>
+        <v>44462.62475694445</v>
       </c>
       <c r="D21" s="2">
-        <v>44456.58785879629</v>
+        <v>44476.62148148148</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>1994</t>
         </is>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Veterinary Science</t>
+          <t>Agriculture</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Private companies</t>
+          <t>There is no main funder as my current research is divided over several different projects with different funders.</t>
         </is>
       </c>
       <c r="J21">
@@ -7051,20 +6797,20 @@
         </is>
       </c>
       <c r="B22">
-        <v>257681865</v>
+        <v>256019631</v>
       </c>
       <c r="C22" s="2">
-        <v>44455.4534375</v>
+        <v>44469.90278935185</v>
       </c>
       <c r="D22" s="2">
-        <v>44452.68805555555</v>
+        <v>44452.90320601852</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1996</t>
         </is>
       </c>
       <c r="G22">
@@ -7072,7 +6818,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>State.</t>
+          <t>Institute</t>
         </is>
       </c>
       <c r="J22">
@@ -7311,28 +7057,28 @@
         </is>
       </c>
       <c r="B23">
-        <v>256233058</v>
+        <v>257040687</v>
       </c>
       <c r="C23" s="2">
-        <v>44452.65792824074</v>
+        <v>44483.56688657407</v>
       </c>
       <c r="D23" s="2">
-        <v>44453.4647337963</v>
+        <v>44469.91393518518</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="G23">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>University funding</t>
+          <t>Public funds</t>
         </is>
       </c>
       <c r="L23">
@@ -7586,22 +7332,6 @@
       </c>
       <c r="GW23">
         <v>3</v>
-      </c>
-      <c r="GY23" t="inlineStr">
-        <is>
-          <t>Agroscope</t>
-        </is>
-      </c>
-      <c r="GZ23" t="inlineStr">
-        <is>
-          <t>Swine research unit</t>
-        </is>
-      </c>
-      <c r="HA23">
-        <v>1</v>
-      </c>
-      <c r="HB23">
-        <v>170</v>
       </c>
     </row>
     <row r="24">
@@ -7611,28 +7341,28 @@
         </is>
       </c>
       <c r="B24">
-        <v>256361947</v>
+        <v>256233058</v>
       </c>
       <c r="C24" s="2">
-        <v>44452.50744212963</v>
+        <v>44470.34854166667</v>
       </c>
       <c r="D24" s="2">
-        <v>44454.530625</v>
+        <v>44470.35540509259</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2004</t>
         </is>
       </c>
       <c r="G24">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Danish Government/ EU</t>
+          <t>DFG</t>
         </is>
       </c>
       <c r="J24">
@@ -7895,12 +7625,6 @@
       </c>
       <c r="GW24">
         <v>3</v>
-      </c>
-      <c r="HA24">
-        <v>2</v>
-      </c>
-      <c r="HB24">
-        <v>65</v>
       </c>
     </row>
     <row r="25">
@@ -7910,33 +7634,23 @@
         </is>
       </c>
       <c r="B25">
-        <v>259543284</v>
+        <v>256542441</v>
       </c>
       <c r="C25" s="2">
-        <v>44452.68103009259</v>
+        <v>44452.65792824074</v>
       </c>
       <c r="D25" s="2">
-        <v>44452.90320601852</v>
+        <v>44467.74414351852</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
       <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>animal science</t>
-        </is>
+        <v>12</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Public funds</t>
+          <t>private companies</t>
         </is>
       </c>
       <c r="J25">
@@ -8166,22 +7880,6 @@
       </c>
       <c r="GW25">
         <v>3</v>
-      </c>
-      <c r="GY25" t="inlineStr">
-        <is>
-          <t>Research Institute for Farm Animal Biology</t>
-        </is>
-      </c>
-      <c r="GZ25" t="inlineStr">
-        <is>
-          <t>Institute of Behavioural Physiology</t>
-        </is>
-      </c>
-      <c r="HA25">
-        <v>1</v>
-      </c>
-      <c r="HB25">
-        <v>65</v>
       </c>
     </row>
     <row r="26">
@@ -8191,29 +7889,24 @@
         </is>
       </c>
       <c r="B26">
-        <v>257626415</v>
+        <v>256361207</v>
       </c>
       <c r="C26" s="2">
         <v>44456.57398148148</v>
       </c>
       <c r="D26" s="2">
-        <v>44470.35540509259</v>
+        <v>44453.36607638889</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="G26">
         <v>2</v>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>I work at a publicly funded research institute, with additional funding mostly from the DFG and EU.</t>
-        </is>
       </c>
       <c r="L26">
         <v>1</v>
@@ -8454,25 +8147,6 @@
       </c>
       <c r="GW26">
         <v>3</v>
-      </c>
-      <c r="GY26" t="inlineStr">
-        <is>
-          <t>IRTA</t>
-        </is>
-      </c>
-      <c r="GZ26" t="inlineStr">
-        <is>
-          <t>Animal Nutrition</t>
-        </is>
-      </c>
-      <c r="HA26">
-        <v>5</v>
-      </c>
-      <c r="HB26">
-        <v>165</v>
-      </c>
-      <c r="HC26">
-        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -8482,25 +8156,28 @@
         </is>
       </c>
       <c r="B27">
-        <v>256339845</v>
+        <v>256558197</v>
       </c>
       <c r="C27" s="2">
-        <v>44467.67358796296</v>
+        <v>44477.46344907407</v>
+      </c>
+      <c r="D27" s="2">
+        <v>44456.58785879629</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
       <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Life sciences</t>
-        </is>
+        <v>8</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Rennes Metropole and #DIGITAG</t>
+          <t>Mineco</t>
         </is>
       </c>
       <c r="L27">
@@ -8535,7 +8212,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>256361207</v>
+        <v>256026620</v>
       </c>
       <c r="C28" s="2">
         <v>44454.486875</v>
@@ -8543,17 +8220,12 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>1996</t>
-        </is>
-      </c>
       <c r="G28">
         <v>12</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Swedish Research Council FORMAS</t>
+          <t>Ministry of Science and Innovation (Spain)</t>
         </is>
       </c>
       <c r="J28">
@@ -8801,22 +8473,6 @@
       </c>
       <c r="GW28">
         <v>3</v>
-      </c>
-      <c r="GY28" t="inlineStr">
-        <is>
-          <t>Inrae</t>
-        </is>
-      </c>
-      <c r="GZ28" t="inlineStr">
-        <is>
-          <t>Pegase</t>
-        </is>
-      </c>
-      <c r="HB28">
-        <v>61</v>
-      </c>
-      <c r="HC28">
-        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -8826,13 +8482,13 @@
         </is>
       </c>
       <c r="B29">
-        <v>256558197</v>
+        <v>256001965</v>
       </c>
       <c r="C29" s="2">
-        <v>44455.40050925926</v>
+        <v>44467.67358796296</v>
       </c>
       <c r="D29" s="2">
-        <v>44456.45372685185</v>
+        <v>44452.54837962963</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -8847,7 +8503,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>There is no main funder as my current research is divided over several different projects with different funders.</t>
+          <t>The Swiss government</t>
         </is>
       </c>
       <c r="J29">
@@ -9026,22 +8682,6 @@
       </c>
       <c r="GW29">
         <v>3</v>
-      </c>
-      <c r="GY29" t="inlineStr">
-        <is>
-          <t>INRAE</t>
-        </is>
-      </c>
-      <c r="GZ29" t="inlineStr">
-        <is>
-          <t>PHASE</t>
-        </is>
-      </c>
-      <c r="HA29">
-        <v>1</v>
-      </c>
-      <c r="HB29">
-        <v>61</v>
       </c>
     </row>
     <row r="30">
@@ -9051,10 +8691,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>255977069</v>
+        <v>259543284</v>
       </c>
       <c r="C30" s="2">
-        <v>44452.51556712963</v>
+        <v>44453.44971064814</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -9069,7 +8709,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>internal university</t>
+          <t>my institute and Europe programs</t>
         </is>
       </c>
       <c r="J30">
@@ -9344,12 +8984,6 @@
       </c>
       <c r="GW30">
         <v>3</v>
-      </c>
-      <c r="HA30">
-        <v>1</v>
-      </c>
-      <c r="HB30">
-        <v>65</v>
       </c>
     </row>
     <row r="31">
@@ -9359,28 +8993,20 @@
         </is>
       </c>
       <c r="B31">
-        <v>256032817</v>
+        <v>257936554</v>
       </c>
       <c r="C31" s="2">
-        <v>44453.44971064814</v>
-      </c>
-      <c r="D31" s="2">
-        <v>44477.46928240741</v>
+        <v>44452.52850694444</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>1994</t>
-        </is>
-      </c>
       <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Goverment</t>
+        <v>12</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Statistics and mathematics</t>
         </is>
       </c>
       <c r="L31">
@@ -9415,33 +9041,23 @@
         </is>
       </c>
       <c r="B32">
-        <v>256064531</v>
+        <v>256337741</v>
       </c>
       <c r="C32" s="2">
-        <v>44455.55013888889</v>
+        <v>44452.62409722222</v>
       </c>
       <c r="D32" s="2">
-        <v>44461.79481481481</v>
+        <v>44467.72538194444</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Not published yet</t>
-        </is>
-      </c>
       <c r="G32">
         <v>2</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Agriculture</t>
-        </is>
-      </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Funds I get for my research are from both public and private sources</t>
+          <t>The Danish Veterinary and Food Administration</t>
         </is>
       </c>
       <c r="K32">
@@ -9599,23 +9215,30 @@
         </is>
       </c>
       <c r="B33">
-        <v>257268868</v>
+        <v>257689731</v>
       </c>
       <c r="C33" s="2">
-        <v>44467.72662037037</v>
-      </c>
-      <c r="D33" s="2">
-        <v>44455.39298611111</v>
+        <v>44452.53380787037</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
       <c r="G33">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>veterinary medicine</t>
+        </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>I work on multiple projects with few weeks or few months for each ... plus some consultancy payed by the department (perhaps from overhead). I am not able to adequately answer this question.</t>
+          <t>Danish Government/ EU</t>
         </is>
       </c>
       <c r="J33">
@@ -9746,13 +9369,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>258745041</v>
+        <v>257131420</v>
       </c>
       <c r="C34" s="2">
-        <v>44454.66171296296</v>
-      </c>
-      <c r="D34" s="2">
-        <v>44453.36607638889</v>
+        <v>44470.73622685185</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -10051,22 +9671,6 @@
       </c>
       <c r="GW34">
         <v>3</v>
-      </c>
-      <c r="GY34" t="inlineStr">
-        <is>
-          <t>INRAE</t>
-        </is>
-      </c>
-      <c r="GZ34" t="inlineStr">
-        <is>
-          <t>UMR PEGASE</t>
-        </is>
-      </c>
-      <c r="HA34">
-        <v>1</v>
-      </c>
-      <c r="HB34">
-        <v>61</v>
       </c>
     </row>
     <row r="35">
@@ -10076,28 +9680,33 @@
         </is>
       </c>
       <c r="B35">
-        <v>256362038</v>
+        <v>256339845</v>
       </c>
       <c r="C35" s="2">
-        <v>44456.50266203703</v>
+        <v>44468.36584490741</v>
       </c>
       <c r="D35" s="2">
-        <v>44467.67511574074</v>
+        <v>44453.4647337963</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>animal science</t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Agroscope, Europe (via ITN)</t>
+          <t>Funds I get for my research are from both public and private sources</t>
         </is>
       </c>
       <c r="L35">
@@ -10351,22 +9960,6 @@
       </c>
       <c r="GW35">
         <v>1</v>
-      </c>
-      <c r="GY35" t="inlineStr">
-        <is>
-          <t>Wageningen University</t>
-        </is>
-      </c>
-      <c r="GZ35" t="inlineStr">
-        <is>
-          <t>department of Animal Science</t>
-        </is>
-      </c>
-      <c r="HA35">
-        <v>4</v>
-      </c>
-      <c r="HB35">
-        <v>123</v>
       </c>
     </row>
     <row r="36">
@@ -10376,23 +9969,30 @@
         </is>
       </c>
       <c r="B36">
-        <v>256019631</v>
+        <v>257620376</v>
       </c>
       <c r="C36" s="2">
-        <v>44476.61056712962</v>
-      </c>
-      <c r="D36" s="2">
-        <v>44483.6057175926</v>
+        <v>44455.40050925926</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
       </c>
       <c r="G36">
         <v>2</v>
       </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Animal health</t>
+        </is>
+      </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Mineco</t>
+          <t>ANR</t>
         </is>
       </c>
       <c r="L36">
@@ -10653,25 +10253,6 @@
         <v>1</v>
       </c>
       <c r="GW36">
-        <v>1</v>
-      </c>
-      <c r="GY36" t="inlineStr">
-        <is>
-          <t>Swedish University of Agricultural Sciences</t>
-        </is>
-      </c>
-      <c r="GZ36" t="inlineStr">
-        <is>
-          <t>Department of Animal Environment and Health</t>
-        </is>
-      </c>
-      <c r="HA36">
-        <v>4</v>
-      </c>
-      <c r="HB36">
-        <v>169</v>
-      </c>
-      <c r="HC36">
         <v>1</v>
       </c>
     </row>
@@ -10682,28 +10263,28 @@
         </is>
       </c>
       <c r="B37">
-        <v>257623952</v>
+        <v>257626517</v>
       </c>
       <c r="C37" s="2">
-        <v>44452.53380787037</v>
+        <v>44455.44020833333</v>
       </c>
       <c r="D37" s="2">
-        <v>44452.54837962963</v>
+        <v>44477.46928240741</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="G37">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>French Government (through the salary)</t>
+          <t>I work on multiple projects with few weeks or few months for each ... plus some consultancy payed by the department (perhaps from overhead). I am not able to adequately answer this question.</t>
         </is>
       </c>
       <c r="J37">
@@ -10993,25 +10574,6 @@
       </c>
       <c r="GW37">
         <v>3</v>
-      </c>
-      <c r="GY37" t="inlineStr">
-        <is>
-          <t>INRAE</t>
-        </is>
-      </c>
-      <c r="GZ37" t="inlineStr">
-        <is>
-          <t>Phase</t>
-        </is>
-      </c>
-      <c r="HA37">
-        <v>5</v>
-      </c>
-      <c r="HB37">
-        <v>61</v>
-      </c>
-      <c r="HC37">
-        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -11024,25 +10586,30 @@
         <v>256331917</v>
       </c>
       <c r="C38" s="2">
-        <v>44452.62409722222</v>
+        <v>44467.67416666666</v>
       </c>
       <c r="D38" s="2">
-        <v>44468.38256944445</v>
+        <v>44455.46857638888</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2002</t>
         </is>
       </c>
       <c r="G38">
         <v>2</v>
       </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Veterinary Science</t>
+        </is>
+      </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>French Government (through the salary)</t>
         </is>
       </c>
       <c r="J38">
@@ -11356,17 +10923,6 @@
       </c>
       <c r="GW38">
         <v>3</v>
-      </c>
-      <c r="GY38" t="inlineStr">
-        <is>
-          <t>Institut de recerca i tecnologia agroalimentaries</t>
-        </is>
-      </c>
-      <c r="HA38">
-        <v>1</v>
-      </c>
-      <c r="HB38">
-        <v>165</v>
       </c>
     </row>
     <row r="39">
@@ -11376,31 +10932,24 @@
         </is>
       </c>
       <c r="B39">
-        <v>255998073</v>
+        <v>257948090</v>
       </c>
       <c r="C39" s="2">
-        <v>44483.56688657407</v>
+        <v>44453.78319444445</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44455.39298611111</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2007</t>
+          <t>Not published yet</t>
         </is>
       </c>
       <c r="G39">
-        <v>12</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Animal Science</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Ministry of Science and Innovation (Spain)</t>
-        </is>
+        <v>2</v>
       </c>
       <c r="U39">
         <v>1</v>
@@ -11527,25 +11076,6 @@
       </c>
       <c r="GW39">
         <v>3</v>
-      </c>
-      <c r="GY39" t="inlineStr">
-        <is>
-          <t>IRTA</t>
-        </is>
-      </c>
-      <c r="GZ39" t="inlineStr">
-        <is>
-          <t>CReSA</t>
-        </is>
-      </c>
-      <c r="HA39">
-        <v>5</v>
-      </c>
-      <c r="HB39">
-        <v>165</v>
-      </c>
-      <c r="HC39">
-        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -11555,17 +11085,20 @@
         </is>
       </c>
       <c r="B40">
-        <v>257634686</v>
+        <v>257268868</v>
       </c>
       <c r="C40" s="2">
-        <v>44468.36584490741</v>
+        <v>44455.55013888889</v>
+      </c>
+      <c r="D40" s="2">
+        <v>44463.87567129629</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2002</t>
+          <t>1988</t>
         </is>
       </c>
       <c r="G40">
@@ -11573,7 +11106,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>My research institute</t>
+          <t>Starting grant</t>
         </is>
       </c>
       <c r="K40">
@@ -11845,22 +11378,6 @@
       </c>
       <c r="GW40">
         <v>1</v>
-      </c>
-      <c r="GY40" t="inlineStr">
-        <is>
-          <t>Swedish University of Agricultural Sciences</t>
-        </is>
-      </c>
-      <c r="GZ40" t="inlineStr">
-        <is>
-          <t>Nutrition and Management</t>
-        </is>
-      </c>
-      <c r="HA40">
-        <v>1</v>
-      </c>
-      <c r="HB40">
-        <v>169</v>
       </c>
     </row>
     <row r="41">
@@ -11870,20 +11387,20 @@
         </is>
       </c>
       <c r="B41">
-        <v>257953342</v>
+        <v>257623952</v>
       </c>
       <c r="C41" s="2">
-        <v>44470.30331018519</v>
+        <v>44467.66538194445</v>
       </c>
       <c r="D41" s="2">
-        <v>44463.87567129629</v>
+        <v>44455.46233796296</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="G41">
@@ -11891,7 +11408,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>The German Government</t>
+          <t>internal university</t>
         </is>
       </c>
       <c r="J41">
@@ -12182,22 +11699,6 @@
       </c>
       <c r="GW41">
         <v>1</v>
-      </c>
-      <c r="GY41" t="inlineStr">
-        <is>
-          <t>Aarhus University</t>
-        </is>
-      </c>
-      <c r="GZ41" t="inlineStr">
-        <is>
-          <t>Animal Science</t>
-        </is>
-      </c>
-      <c r="HA41">
-        <v>3</v>
-      </c>
-      <c r="HB41">
-        <v>47</v>
       </c>
     </row>
     <row r="42">
@@ -12207,28 +11708,28 @@
         </is>
       </c>
       <c r="B42">
-        <v>256001965</v>
+        <v>256081511</v>
       </c>
       <c r="C42" s="2">
-        <v>44467.65208333333</v>
+        <v>44452.51556712963</v>
       </c>
       <c r="D42" s="2">
-        <v>44476.62148148148</v>
+        <v>44470.31486111111</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>1989</t>
         </is>
       </c>
       <c r="G42">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Europe Funds</t>
+          <t>National research instute for my salary and europe for my research</t>
         </is>
       </c>
       <c r="J42">
@@ -12479,22 +11980,6 @@
       </c>
       <c r="GW42">
         <v>3</v>
-      </c>
-      <c r="GY42" t="inlineStr">
-        <is>
-          <t>FBN - Dummerstorf</t>
-        </is>
-      </c>
-      <c r="GZ42" t="inlineStr">
-        <is>
-          <t>Nutritional Physiology</t>
-        </is>
-      </c>
-      <c r="HA42">
-        <v>3</v>
-      </c>
-      <c r="HB42">
-        <v>65</v>
       </c>
     </row>
     <row r="43">
@@ -12504,23 +11989,28 @@
         </is>
       </c>
       <c r="B43">
-        <v>256324567</v>
+        <v>256171924</v>
       </c>
       <c r="C43" s="2">
-        <v>44455.55667824074</v>
+        <v>44468.39248842592</v>
       </c>
       <c r="D43" s="2">
-        <v>44468.41116898148</v>
+        <v>44456.51704861112</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
       <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Animal nutrition</t>
+        <v>12</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Public funder</t>
         </is>
       </c>
       <c r="J43">
@@ -12738,22 +12228,6 @@
       </c>
       <c r="GW43">
         <v>3</v>
-      </c>
-      <c r="GY43" t="inlineStr">
-        <is>
-          <t>IRTA</t>
-        </is>
-      </c>
-      <c r="GZ43" t="inlineStr">
-        <is>
-          <t>Animal Nutrition</t>
-        </is>
-      </c>
-      <c r="HA43">
-        <v>5</v>
-      </c>
-      <c r="HB43">
-        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>